<commit_message>
Final minor edits to metadata descriptions to improve clarity
</commit_message>
<xml_diff>
--- a/data/Penczykowski_et_al_BagExptData_Metadata.xlsx
+++ b/data/Penczykowski_et_al_BagExptData_Metadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://umich-my.sharepoint.com/personal/mlfearon_umich_edu/Documents/PROJECTS/Manuscripts/Parasitism alters effects of mixing and nutrients - Oecologia/Data and Code/nutrient-bag-expt/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="11_DAE24148930A6AEF961DA7A0D216E75A32FB9A6E" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5CB3AB7C-D727-40DA-ACF7-91B810EB98D0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{A16437C5-B792-417D-823F-58CB9B2C2CDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3780" yWindow="1560" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31020" yWindow="1830" windowWidth="21600" windowHeight="11265" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="69">
   <si>
     <t>Raft</t>
   </si>
@@ -84,9 +84,6 @@
     <t>Units</t>
   </si>
   <si>
-    <t>32 bags total (4 replicates x 8 treatments)</t>
-  </si>
-  <si>
     <t>μg/L</t>
   </si>
   <si>
@@ -111,12 +108,6 @@
     <t>Bags were suspended from rafts. There were 4 rafts, each with 1 replicate of each of the 8 treatments (i.e., rafts = "blocks")</t>
   </si>
   <si>
-    <t>Sampling days numbered 1 through 15 (i.e., pretending the time intervals are evenly spaced)</t>
-  </si>
-  <si>
-    <t>Reference</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Parasite treatment in which </t>
     </r>
@@ -462,24 +453,6 @@
     <t>LogTN</t>
   </si>
   <si>
-    <t>Log of Total phosphorus (added 1 to TP with a value of zero to allow for the log transformation)</t>
-  </si>
-  <si>
-    <t>Log of Total nitrogen (added 1 to TN with a value of zero to allow for the log transformation)</t>
-  </si>
-  <si>
-    <t>Log of Total Denisity (added 1 to Total Density with a value of zero to allow for the log transformation)</t>
-  </si>
-  <si>
-    <t>Log of Uninfected Denisity (added 1 to Uninfected Density with a value of zero to allow for the log transformation)</t>
-  </si>
-  <si>
-    <t>Log of Infected Denisity (added 1 to Infected Density with a value of zero to allow for the log transformation)</t>
-  </si>
-  <si>
-    <t>Log of Edible Chl (added 1 to Edible Chl with a value of zero to allow for the log transformation)</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Number of all uninfected </t>
     </r>
@@ -719,6 +692,30 @@
   </si>
   <si>
     <t>%</t>
+  </si>
+  <si>
+    <t>32 bags total (4 replicates x 8 treatments); note that a total of five bags are excluded from analysis (and from this dataset), as explained in the methods section of the manuscript</t>
+  </si>
+  <si>
+    <t>Sampling days numbered 1 through 15 (i.e., order of sampling days rather than actual time intervals)</t>
+  </si>
+  <si>
+    <t>Log-transformed TotalDensity (added 1 to TotalDensity with a value of zero to allow for the log transformation)</t>
+  </si>
+  <si>
+    <t>Log-transformed UninfDensity (added 1 to UninfDensity with a value of zero to allow for the log transformation)</t>
+  </si>
+  <si>
+    <t>Log-tranformed InfDensity (added 1 to InfDensity with a value of zero to allow for the log transformation)</t>
+  </si>
+  <si>
+    <t>Log-transformed EdChl (there were no zero values for EdChl)</t>
+  </si>
+  <si>
+    <t>Log-transformed TP (there were no zero values for TP)</t>
+  </si>
+  <si>
+    <t>Log-transformed TN (there were no zero values for TN)</t>
   </si>
 </sst>
 </file>
@@ -1062,22 +1059,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D32"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="104.5703125" style="2" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.7109375" style="2"/>
+    <col min="2" max="2" width="112.140625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="16384" width="8.7109375" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>16</v>
       </c>
@@ -1087,149 +1083,146 @@
       <c r="C1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1237,10 +1230,10 @@
         <v>13</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1248,10 +1241,10 @@
         <v>14</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1259,135 +1252,135 @@
         <v>15</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>53</v>
+        <v>50</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>55</v>
+        <v>67</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>54</v>
+        <v>51</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>56</v>
+        <v>68</v>
       </c>
     </row>
   </sheetData>

</xml_diff>